<commit_message>
added codex, codex items, folio generators, generated all cards
</commit_message>
<xml_diff>
--- a/Scripts/python/SourceTables/CodexItems.xlsx
+++ b/Scripts/python/SourceTables/CodexItems.xlsx
@@ -36,9 +36,6 @@
     <t>8307</t>
   </si>
   <si>
-    <t>Часть: Лазурное небо</t>
-  </si>
-  <si>
     <t>Часть кодекса</t>
   </si>
   <si>
@@ -138,36 +135,24 @@
     <t>Веды 2 ур.</t>
   </si>
   <si>
-    <t>Случайный кодекс 2 ур.: Железная воля, Цветки алычи, Красный лотос, Злоумышленник, Сказ о персиках, Под стеной, Пламя дум, Гид по волкам.</t>
-  </si>
-  <si>
     <t>8103</t>
   </si>
   <si>
     <t>Веды 3 ур.</t>
   </si>
   <si>
-    <t>Случайный кодекс 3 ур.: Пир, Байки заката, Багрянец, Горный проход, Байки красоты, Минор, Раздумья поэта, Коллапс.</t>
-  </si>
-  <si>
     <t>8104</t>
   </si>
   <si>
     <t>Веды 4 ур.</t>
   </si>
   <si>
-    <t>Случайный кодекс 4 ур.: Боевые тактики, Страсть, Судьба, Шип розы, Весенний голод, Потрясение, Юг реки.</t>
-  </si>
-  <si>
     <t>8105</t>
   </si>
   <si>
     <t>Скрипт судьбы</t>
   </si>
   <si>
-    <t>Случайный кодекс 5 ур.: Ярость небес, Аромат, Разлука, Рия и алые губы, Вечные волны, Хулиганы, Сад пустоты.</t>
-  </si>
-  <si>
     <t>8106</t>
   </si>
   <si>
@@ -204,18 +189,12 @@
     <t>8112</t>
   </si>
   <si>
-    <t>Часть: "Тоска"</t>
-  </si>
-  <si>
     <t>Из 50 частей «Тоски» можно синтезировать в горне Кодекс «Тоска» 4 ур.</t>
   </si>
   <si>
     <t>8114</t>
   </si>
   <si>
-    <t>Часть: Буря</t>
-  </si>
-  <si>
     <t>Из 20 частей «Бури» можно синтезировать в горне кодекс «Буря» 6 ур.</t>
   </si>
   <si>
@@ -240,40 +219,96 @@
     <t>Из 6 листов кодекса в Сумке &gt; Горне синтезируется случайный кодекс 1 ур.</t>
   </si>
   <si>
-    <t>Из 4 частей можно синтезировать фолиант: Лазурное небо.\n\nПосле синтеза фолиант будет добавлен в коллекцию. Просмотр: Кодекс &gt; Сутра\n\nФолиант можно добавить в коллекцию только 1 раз.</t>
-  </si>
-  <si>
-    <t>Открывает и улучшает созвездие кодекса: Созвездие начала\n\nБазовые характеристики:\n● С каждым уровнем увеличивает HP персонажа\n● С каждым уровнем увеличивает АТК персонажа\n\nОбычное созвездие, не обладает большой мощью, но подходит для каждого поля боя.</t>
-  </si>
-  <si>
-    <t>Открывает и улучшает созвездие кодекса: Созвездие Дуо\n\nБазовые характеристики:\n● Буйство: с каждым уровнем увеличивает урон по монстрам\n● Эгида: с каждым уровнем снижает урон от монстров\n● Рекурсия: повышает характеристики кодекса на 30%\n● Суд: снижает характеристики кодекса на 30%\n\nЭлитное созвездие, незаменимо в борьбе с монстрами.</t>
-  </si>
-  <si>
-    <t>Открывает и улучшает созвездие кодекса: Созвездие Трио\n\nБазовые характеристики:\n● Злость: с каждым уровнем увеличивает урон по игрокам\n● Стойкость: с каждым уровнем снижает урон от игроков\n● Эфир: повышает навык кодекса на 1 ур.\n● Погибель: снижает навык кодекса на 1 ур.\n\nЭлитное созвездие, незаменимо в борьбе с игроками.</t>
-  </si>
-  <si>
-    <t>Улучшение созвездия кодекса Созвездие Дуо 10 ур и выше\n\nНа 15 ур открывается 5-й слот для кодекса\n\nМожно разобрать на Генезис х1.</t>
-  </si>
-  <si>
-    <t>Улучшение созвездия кодекса Созвездие Трио 10 ур и выше\n\nНа 15 ур открывается 5-й слот для кодекса\n\nМожно разобрать на Генезис х1.</t>
-  </si>
-  <si>
-    <t>С помощью этого предмета во время улучшения Книги небес можно получить опыт x1,5\nПримените здесь: Кодекс &gt; Свитки &gt; Книга небес.\n\nВ книге записываются небесные явления и карты мистических мест.</t>
-  </si>
-  <si>
-    <t>С помощью этого предмета во время улучшения Книги небес можно получить опыт x2.\nПримените здесь: Кодекс &gt; Свитки &gt; Книга небес.\n\nВ книге записываются небесные явления и карты мистических мест.</t>
-  </si>
-  <si>
-    <t>Предмет для развития Свитка кодекса.\nПримените здесь: Кодекс &gt; Свитки &gt; Свитки.\n\nДревний свиток, появившийся в незапамятные времена.</t>
-  </si>
-  <si>
-    <t>Из 25 частей руны кодекса 6 ур. можно синтезировать в горне руну кодекса 6 ур. Руна дает на выбор «Возмездие» или «Покровительство». Все предметы персональные.\n\nМожно получить, купив в Магазине временный тюк.</t>
-  </si>
-  <si>
-    <t>Дает лист кодекса и случайный кодекс 1 ур.: Утес, Полет духа, Огонь греха, Небесный гигант, Наступление, Великан, Грациозность, Куст.\n\nКодексы доступны с 55 ур.</t>
-  </si>
-  <si>
-    <t>Дает Лист кодекса х10.\nШанс получить одну из наград:\n●Кодекс 1 ур.: Полет духа, Огонь греха, Небесный гигант, Наступление, Великан, Грациозность, Куст, Утес.\n●Кодекс 2 ур.: Железная воля, Цветки алычи, Красный лотос, Злоумышленник, Сказ о персиках, Под стеной, Пламя дум, Гид по волкам.\n●Кодекс 3 ур.: Пир, Байки заката, Багрянец, Горный проход, Байки красоты, Минор, Раздумья поэта, Коллапс.\n\nКодексы доступны с 55 ур.</t>
+    <t>Улучшение созвездия кодекса Созвездие Дуо 10 ур и выше
+На 15 ур открывается 5-й слот для кодекса
+Можно разобрать на Генезис х1.</t>
+  </si>
+  <si>
+    <t>Улучшение созвездия кодекса Созвездие Трио 10 ур и выше
+На 15 ур открывается 5-й слот для кодекса
+Можно разобрать на Генезис х1.</t>
+  </si>
+  <si>
+    <t>Из 25 частей руны кодекса 6 ур. можно синтезировать в горне руну кодекса 6 ур. Руна дает на выбор «Возмездие» или «Покровительство». Все предметы персональные.
+Можно получить, купив в Магазине временный тюк.</t>
+  </si>
+  <si>
+    <t>Часть Лазурное небо</t>
+  </si>
+  <si>
+    <t>Из 4 частей можно синтезировать фолиант Лазурное небо.
+После синтеза фолиант будет добавлен в коллекцию. Просмотр Кодекс &gt; Сутра
+Фолиант можно добавить в коллекцию только 1 раз.</t>
+  </si>
+  <si>
+    <t>Открывает и улучшает созвездие кодекса Созвездие начала
+Базовые характеристики
+● С каждым уровнем увеличивает HP персонажа
+● С каждым уровнем увеличивает АТК персонажа
+Обычное созвездие, не обладает большой мощью, но подходит для каждого поля боя.</t>
+  </si>
+  <si>
+    <t>Открывает и улучшает созвездие кодекса Созвездие Дуо
+Базовые характеристики
+● Буйство с каждым уровнем увеличивает урон по монстрам
+● Эгида с каждым уровнем снижает урон от монстров
+● Рекурсия повышает характеристики кодекса на 30%
+● Суд снижает характеристики кодекса на 30%
+Элитное созвездие, незаменимо в борьбе с монстрами.</t>
+  </si>
+  <si>
+    <t>Открывает и улучшает созвездие кодекса Созвездие Трио
+Базовые характеристики
+● Злость с каждым уровнем увеличивает урон по игрокам
+● Стойкость с каждым уровнем снижает урон от игроков
+● Эфир повышает навык кодекса на 1 ур.
+● Погибель снижает навык кодекса на 1 ур.
+Элитное созвездие, незаменимо в борьбе с игроками.</t>
+  </si>
+  <si>
+    <t>С помощью этого предмета во время улучшения Книги небес можно получить опыт x1,5
+Примените здесь Кодекс &gt; Свитки &gt; Книга небес.
+В книге записываются небесные явления и карты мистических мест.</t>
+  </si>
+  <si>
+    <t>С помощью этого предмета во время улучшения Книги небес можно получить опыт x2.
+Примените здесь Кодекс &gt; Свитки &gt; Книга небес.
+В книге записываются небесные явления и карты мистических мест.</t>
+  </si>
+  <si>
+    <t>Предмет для развития Свитка кодекса.
+Примените здесь Кодекс &gt; Свитки &gt; Свитки.
+Древний свиток, появившийся в незапамятные времена.</t>
+  </si>
+  <si>
+    <t>Дает лист кодекса и случайный кодекс 1 ур. Утес, Полет духа, Огонь греха, Небесный гигант, Наступление, Великан, Грациозность, Куст.
+Кодексы доступны с 55 ур.</t>
+  </si>
+  <si>
+    <t>Случайный кодекс 2 ур. Железная воля, Цветки алычи, Красный лотос, Злоумышленник, Сказ о персиках, Под стеной, Пламя дум, Гид по волкам.</t>
+  </si>
+  <si>
+    <t>Случайный кодекс 3 ур. Пир, Байки заката, Багрянец, Горный проход, Байки красоты, Минор, Раздумья поэта, Коллапс.</t>
+  </si>
+  <si>
+    <t>Случайный кодекс 4 ур. Боевые тактики, Страсть, Судьба, Шип розы, Весенний голод, Потрясение, Юг реки.</t>
+  </si>
+  <si>
+    <t>Случайный кодекс 5 ур. Ярость небес, Аромат, Разлука, Рия и алые губы, Вечные волны, Хулиганы, Сад пустоты.</t>
+  </si>
+  <si>
+    <t>Дает Лист кодекса х10.
+Шанс получить одну из наград
+●Кодекс 1 ур. Полет духа, Огонь греха, Небесный гигант, Наступление, Великан, Грациозность, Куст, Утес.
+●Кодекс 2 ур. Железная воля, Цветки алычи, Красный лотос, Злоумышленник, Сказ о персиках, Под стеной, Пламя дум, Гид по волкам.
+●Кодекс 3 ур. Пир, Байки заката, Багрянец, Горный проход, Байки красоты, Минор, Раздумья поэта, Коллапс.
+Кодексы доступны с 55 ур.</t>
+  </si>
+  <si>
+    <t>Часть Буря</t>
+  </si>
+  <si>
+    <t>Часть Тоска</t>
   </si>
 </sst>
 </file>
@@ -393,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,6 +440,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -713,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,382 +775,382 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="99" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="132" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="6" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="9" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="115.5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="181.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>